<commit_message>
Major updates for prototype
</commit_message>
<xml_diff>
--- a/cellplans/telcel.xlsx
+++ b/cellplans/telcel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520"/>
@@ -672,10 +672,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;MX$&quot;* #,##0.00_);_(&quot;MX$&quot;* \(#,##0.00\);_(&quot;MX$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;MX$&quot;* #,##0.00_);_(&quot;MX$&quot;* \(#,##0.00\);_(&quot;MX$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -862,1249 +862,1249 @@
   </borders>
   <cellStyleXfs count="1449">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2343,11 +2343,11 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1243" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="1243" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="1242" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="1243" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="1242" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="1243" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2365,8 +2365,8 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1242" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="1242" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2388,10 +2388,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1412" applyFont="1"/>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1412" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="5" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="1412" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1412" applyFont="1"/>
@@ -2402,8 +2402,8 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1412" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="1412" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="1" fillId="6" borderId="0" xfId="1412" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="0" xfId="1412" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1449">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8" hidden="1"/>
@@ -4347,7 +4347,7 @@
   <dimension ref="A1:AS42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
@@ -10028,7 +10028,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -10875,7 +10874,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -11401,7 +11399,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>